<commit_message>
Adding support for FFT
(1) Adding FFTW library
(2) Refactored some code
(3) Adding blank classes to implement Variance Gamma Method
</commit_message>
<xml_diff>
--- a/Results/CalendarSpreadBounds.xlsx
+++ b/Results/CalendarSpreadBounds.xlsx
@@ -48,6 +48,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -79,7 +82,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,7 +350,7 @@
             <c:numRef>
               <c:f>CalendarSpreadBounds!$B$2:$B$42</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>6.67853E-13</c:v>
@@ -358,118 +361,118 @@
                 <c:pt idx="2">
                   <c:v>1.96501E-5</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>0.000549776</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>0.00527118</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>0.0272357</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>0.0949404</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>0.253242</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>0.558122</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="9">
                   <c:v>1.06816</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>1.83626</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>2.90383</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>4.29804</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>6.0316</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>8.10433</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>10.5016</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>13.1561</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>15.7981</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>17.8496</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>18.7925</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>18.6776</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="General">
+                <c:pt idx="21">
                   <c:v>17.9869</c:v>
                 </c:pt>
-                <c:pt idx="22" formatCode="General">
+                <c:pt idx="22">
                   <c:v>17.151</c:v>
                 </c:pt>
-                <c:pt idx="23" formatCode="General">
+                <c:pt idx="23">
                   <c:v>16.3681</c:v>
                 </c:pt>
-                <c:pt idx="24" formatCode="General">
+                <c:pt idx="24">
                   <c:v>15.6877</c:v>
                 </c:pt>
-                <c:pt idx="25" formatCode="General">
+                <c:pt idx="25">
                   <c:v>15.108</c:v>
                 </c:pt>
-                <c:pt idx="26" formatCode="General">
+                <c:pt idx="26">
                   <c:v>14.6165</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="General">
+                <c:pt idx="27">
                   <c:v>14.2006</c:v>
                 </c:pt>
-                <c:pt idx="28" formatCode="General">
+                <c:pt idx="28">
                   <c:v>13.8489</c:v>
                 </c:pt>
-                <c:pt idx="29" formatCode="General">
+                <c:pt idx="29">
                   <c:v>13.5517</c:v>
                 </c:pt>
-                <c:pt idx="30" formatCode="General">
+                <c:pt idx="30">
                   <c:v>13.3006</c:v>
                 </c:pt>
-                <c:pt idx="31" formatCode="General">
+                <c:pt idx="31">
                   <c:v>13.0886</c:v>
                 </c:pt>
-                <c:pt idx="32" formatCode="General">
+                <c:pt idx="32">
                   <c:v>12.9096</c:v>
                 </c:pt>
-                <c:pt idx="33" formatCode="General">
+                <c:pt idx="33">
                   <c:v>12.7584</c:v>
                 </c:pt>
-                <c:pt idx="34" formatCode="General">
+                <c:pt idx="34">
                   <c:v>12.6308</c:v>
                 </c:pt>
-                <c:pt idx="35" formatCode="General">
+                <c:pt idx="35">
                   <c:v>12.5229</c:v>
                 </c:pt>
-                <c:pt idx="36" formatCode="General">
+                <c:pt idx="36">
                   <c:v>12.4318</c:v>
                 </c:pt>
-                <c:pt idx="37" formatCode="General">
+                <c:pt idx="37">
                   <c:v>12.3548</c:v>
                 </c:pt>
-                <c:pt idx="38" formatCode="General">
+                <c:pt idx="38">
                   <c:v>12.2896</c:v>
                 </c:pt>
-                <c:pt idx="39" formatCode="General">
+                <c:pt idx="39">
                   <c:v>12.2345</c:v>
                 </c:pt>
-                <c:pt idx="40" formatCode="General">
+                <c:pt idx="40">
                   <c:v>12.1878</c:v>
                 </c:pt>
               </c:numCache>
@@ -640,9 +643,9 @@
             <c:numRef>
               <c:f>CalendarSpreadBounds!$C$2:$C$42</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="41"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -660,109 +663,109 @@
                 <c:pt idx="5">
                   <c:v>-5.05446E-5</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>-0.000581521</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>-0.00388098</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>-0.0175655</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="9">
                   <c:v>-0.0596733</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>-0.163029</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>-0.375808</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>-0.752699</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>-1.31378</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>-1.94314</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>-2.31971</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>-2.07294</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>-1.07486</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>0.476507</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>2.24381</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>3.95555</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="General">
+                <c:pt idx="21">
                   <c:v>5.47248</c:v>
                 </c:pt>
-                <c:pt idx="22" formatCode="General">
+                <c:pt idx="22">
                   <c:v>6.75481</c:v>
                 </c:pt>
-                <c:pt idx="23" formatCode="General">
+                <c:pt idx="23">
                   <c:v>7.81207</c:v>
                 </c:pt>
-                <c:pt idx="24" formatCode="General">
+                <c:pt idx="24">
                   <c:v>8.67137</c:v>
                 </c:pt>
-                <c:pt idx="25" formatCode="General">
+                <c:pt idx="25">
                   <c:v>9.36308</c:v>
                 </c:pt>
-                <c:pt idx="26" formatCode="General">
+                <c:pt idx="26">
                   <c:v>9.91577</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="General">
+                <c:pt idx="27">
                   <c:v>10.3546</c:v>
                 </c:pt>
-                <c:pt idx="28" formatCode="General">
+                <c:pt idx="28">
                   <c:v>10.7012</c:v>
                 </c:pt>
-                <c:pt idx="29" formatCode="General">
+                <c:pt idx="29">
                   <c:v>10.9737</c:v>
                 </c:pt>
-                <c:pt idx="30" formatCode="General">
+                <c:pt idx="30">
                   <c:v>11.187</c:v>
                 </c:pt>
-                <c:pt idx="31" formatCode="General">
+                <c:pt idx="31">
                   <c:v>11.3533</c:v>
                 </c:pt>
-                <c:pt idx="32" formatCode="General">
+                <c:pt idx="32">
                   <c:v>11.4827</c:v>
                 </c:pt>
-                <c:pt idx="33" formatCode="General">
+                <c:pt idx="33">
                   <c:v>11.583</c:v>
                 </c:pt>
-                <c:pt idx="34" formatCode="General">
+                <c:pt idx="34">
                   <c:v>11.6607</c:v>
                 </c:pt>
-                <c:pt idx="35" formatCode="General">
+                <c:pt idx="35">
                   <c:v>11.7206</c:v>
                 </c:pt>
-                <c:pt idx="36" formatCode="General">
+                <c:pt idx="36">
                   <c:v>11.7668</c:v>
                 </c:pt>
-                <c:pt idx="37" formatCode="General">
+                <c:pt idx="37">
                   <c:v>11.8024</c:v>
                 </c:pt>
-                <c:pt idx="38" formatCode="General">
+                <c:pt idx="38">
                   <c:v>11.8298</c:v>
                 </c:pt>
-                <c:pt idx="39" formatCode="General">
+                <c:pt idx="39">
                   <c:v>11.8508</c:v>
                 </c:pt>
-                <c:pt idx="40" formatCode="General">
+                <c:pt idx="40">
                   <c:v>11.867</c:v>
                 </c:pt>
               </c:numCache>
@@ -933,7 +936,7 @@
             <c:numRef>
               <c:f>CalendarSpreadBounds!$D$2:$D$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -941,16 +944,16 @@
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00E+00">
+                <c:pt idx="2">
                   <c:v>1.9541E-12</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
+                <c:pt idx="3">
                   <c:v>4.97995E-9</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
+                <c:pt idx="4">
                   <c:v>9.15578E-7</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
+                <c:pt idx="5">
                   <c:v>3.71839E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
@@ -1225,7 +1228,7 @@
             <c:numRef>
               <c:f>CalendarSpreadBounds!$E$2:$E$42</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>4.61652E-14</c:v>
@@ -1236,118 +1239,118 @@
                 <c:pt idx="2">
                   <c:v>1.42509E-5</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>0.000459231</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>0.004919</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>0.0256446</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>0.0922933</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>0.252344</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>0.544379</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="9">
                   <c:v>1.05262</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>1.79384</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>2.79006</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>4.03738</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>5.50148</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>7.1356</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>8.95444</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>10.7962</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>12.8361</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>14.4464</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>15.4047</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>15.5765</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="General">
+                <c:pt idx="21">
                   <c:v>15.4089</c:v>
                 </c:pt>
-                <c:pt idx="22" formatCode="General">
+                <c:pt idx="22">
                   <c:v>15.0502</c:v>
                 </c:pt>
-                <c:pt idx="23" formatCode="General">
+                <c:pt idx="23">
                   <c:v>14.7202</c:v>
                 </c:pt>
-                <c:pt idx="24" formatCode="General">
+                <c:pt idx="24">
                   <c:v>14.4177</c:v>
                 </c:pt>
-                <c:pt idx="25" formatCode="General">
+                <c:pt idx="25">
                   <c:v>14.1362</c:v>
                 </c:pt>
-                <c:pt idx="26" formatCode="General">
+                <c:pt idx="26">
                   <c:v>13.8841</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="General">
+                <c:pt idx="27">
                   <c:v>13.6464</c:v>
                 </c:pt>
-                <c:pt idx="28" formatCode="General">
+                <c:pt idx="28">
                   <c:v>13.4115</c:v>
                 </c:pt>
-                <c:pt idx="29" formatCode="General">
+                <c:pt idx="29">
                   <c:v>13.1939</c:v>
                 </c:pt>
-                <c:pt idx="30" formatCode="General">
+                <c:pt idx="30">
                   <c:v>13.0394</c:v>
                 </c:pt>
-                <c:pt idx="31" formatCode="General">
+                <c:pt idx="31">
                   <c:v>12.8901</c:v>
                 </c:pt>
-                <c:pt idx="32" formatCode="General">
+                <c:pt idx="32">
                   <c:v>12.7639</c:v>
                 </c:pt>
-                <c:pt idx="33" formatCode="General">
+                <c:pt idx="33">
                   <c:v>12.6458</c:v>
                 </c:pt>
-                <c:pt idx="34" formatCode="General">
+                <c:pt idx="34">
                   <c:v>12.5324</c:v>
                 </c:pt>
-                <c:pt idx="35" formatCode="General">
+                <c:pt idx="35">
                   <c:v>12.4555</c:v>
                 </c:pt>
-                <c:pt idx="36" formatCode="General">
+                <c:pt idx="36">
                   <c:v>12.3859</c:v>
                 </c:pt>
-                <c:pt idx="37" formatCode="General">
+                <c:pt idx="37">
                   <c:v>12.3049</c:v>
                 </c:pt>
-                <c:pt idx="38" formatCode="General">
+                <c:pt idx="38">
                   <c:v>12.2575</c:v>
                 </c:pt>
-                <c:pt idx="39" formatCode="General">
+                <c:pt idx="39">
                   <c:v>12.2117</c:v>
                 </c:pt>
-                <c:pt idx="40" formatCode="General">
+                <c:pt idx="40">
                   <c:v>12.1629</c:v>
                 </c:pt>
               </c:numCache>
@@ -1517,7 +1520,7 @@
             <c:numRef>
               <c:f>CalendarSpreadBounds!$F$2:$F$42</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>3.65678E-85</c:v>
@@ -1552,94 +1555,94 @@
                 <c:pt idx="10">
                   <c:v>2.45126E-5</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.000676778</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.00888636</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.0655499</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.347244</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.11323</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>2.32046</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>3.58746</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>4.77761</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>5.85796</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>6.87358</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="General">
+                <c:pt idx="21">
                   <c:v>7.72729</c:v>
                 </c:pt>
-                <c:pt idx="22" formatCode="General">
+                <c:pt idx="22">
                   <c:v>8.53202</c:v>
                 </c:pt>
-                <c:pt idx="23" formatCode="General">
+                <c:pt idx="23">
                   <c:v>9.12971</c:v>
                 </c:pt>
-                <c:pt idx="24" formatCode="General">
+                <c:pt idx="24">
                   <c:v>9.70899</c:v>
                 </c:pt>
-                <c:pt idx="25" formatCode="General">
+                <c:pt idx="25">
                   <c:v>10.1173</c:v>
                 </c:pt>
-                <c:pt idx="26" formatCode="General">
+                <c:pt idx="26">
                   <c:v>10.5223</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="General">
+                <c:pt idx="27">
                   <c:v>10.7826</c:v>
                 </c:pt>
-                <c:pt idx="28" formatCode="General">
+                <c:pt idx="28">
                   <c:v>11.0512</c:v>
                 </c:pt>
-                <c:pt idx="29" formatCode="General">
+                <c:pt idx="29">
                   <c:v>11.216</c:v>
                 </c:pt>
-                <c:pt idx="30" formatCode="General">
+                <c:pt idx="30">
                   <c:v>11.375</c:v>
                 </c:pt>
-                <c:pt idx="31" formatCode="General">
+                <c:pt idx="31">
                   <c:v>11.5052</c:v>
                 </c:pt>
-                <c:pt idx="32" formatCode="General">
+                <c:pt idx="32">
                   <c:v>11.5879</c:v>
                 </c:pt>
-                <c:pt idx="33" formatCode="General">
+                <c:pt idx="33">
                   <c:v>11.6746</c:v>
                 </c:pt>
-                <c:pt idx="34" formatCode="General">
+                <c:pt idx="34">
                   <c:v>11.7242</c:v>
                 </c:pt>
-                <c:pt idx="35" formatCode="General">
+                <c:pt idx="35">
                   <c:v>11.7673</c:v>
                 </c:pt>
-                <c:pt idx="36" formatCode="General">
+                <c:pt idx="36">
                   <c:v>11.8106</c:v>
                 </c:pt>
-                <c:pt idx="37" formatCode="General">
+                <c:pt idx="37">
                   <c:v>11.8305</c:v>
                 </c:pt>
-                <c:pt idx="38" formatCode="General">
+                <c:pt idx="38">
                   <c:v>11.8507</c:v>
                 </c:pt>
-                <c:pt idx="39" formatCode="General">
+                <c:pt idx="39">
                   <c:v>11.8711</c:v>
                 </c:pt>
-                <c:pt idx="40" formatCode="General">
+                <c:pt idx="40">
                   <c:v>11.8803</c:v>
                 </c:pt>
               </c:numCache>
@@ -1655,11 +1658,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2052248464"/>
-        <c:axId val="-2005081568"/>
+        <c:axId val="-2054082592"/>
+        <c:axId val="-2070184112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2052248464"/>
+        <c:axId val="-2054082592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,12 +1780,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005081568"/>
+        <c:crossAx val="-2070184112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2005081568"/>
+        <c:axId val="-2070184112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1863,7 +1866,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1900,7 +1903,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2052248464"/>
+        <c:crossAx val="-2054082592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2838,7 +2841,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2870,10 +2873,10 @@
       <c r="B2" s="1">
         <v>6.6785300000000004E-13</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
       <c r="E2" s="1">
@@ -2893,7 +2896,7 @@
       <c r="C3" s="1">
         <v>-1.93945E-15</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1">
@@ -2927,7 +2930,7 @@
       <c r="A5">
         <v>20</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>5.4977599999999998E-4</v>
       </c>
       <c r="C5" s="1">
@@ -2936,7 +2939,7 @@
       <c r="D5" s="1">
         <v>4.9799500000000004E-9</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>4.5923099999999999E-4</v>
       </c>
       <c r="F5" s="1">
@@ -2947,7 +2950,7 @@
       <c r="A6">
         <v>25</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>5.2711800000000003E-3</v>
       </c>
       <c r="C6" s="1">
@@ -2956,7 +2959,7 @@
       <c r="D6" s="1">
         <v>9.1557799999999999E-7</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>4.9189999999999998E-3</v>
       </c>
       <c r="F6" s="1">
@@ -2967,7 +2970,7 @@
       <c r="A7">
         <v>30</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>2.7235700000000002E-2</v>
       </c>
       <c r="C7" s="1">
@@ -2976,7 +2979,7 @@
       <c r="D7" s="1">
         <v>3.7183900000000002E-5</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>2.56446E-2</v>
       </c>
       <c r="F7" s="1">
@@ -2987,16 +2990,16 @@
       <c r="A8">
         <v>35</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>9.4940399999999994E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>-5.8152099999999999E-4</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>5.8057300000000003E-4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>9.2293299999999995E-2</v>
       </c>
       <c r="F8" s="1">
@@ -3007,16 +3010,16 @@
       <c r="A9">
         <v>40</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>0.25324200000000002</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>-3.88098E-3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>4.7509600000000003E-3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>0.25234400000000001</v>
       </c>
       <c r="F9" s="1">
@@ -3027,16 +3030,16 @@
       <c r="A10">
         <v>45</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.55812200000000001</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>-1.7565500000000001E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>2.4598499999999999E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>0.54437899999999995</v>
       </c>
       <c r="F10" s="1">
@@ -3047,16 +3050,16 @@
       <c r="A11">
         <v>50</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1.06816</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>-5.9673299999999999E-2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>9.0960399999999997E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>1.0526199999999999</v>
       </c>
       <c r="F11" s="1">
@@ -3067,16 +3070,16 @@
       <c r="A12">
         <v>55</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>1.83626</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>-0.16302900000000001</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>0.26045699999999999</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>1.7938400000000001</v>
       </c>
       <c r="F12" s="1">
@@ -3087,19 +3090,19 @@
       <c r="A13">
         <v>60</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>2.9038300000000001</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>-0.37580799999999998</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>0.61035600000000001</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>2.79006</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>6.7677799999999995E-4</v>
       </c>
     </row>
@@ -3107,19 +3110,19 @@
       <c r="A14">
         <v>65</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>4.2980400000000003</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>-0.75269900000000001</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>1.2168600000000001</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>4.0373799999999997</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>8.8863599999999994E-3</v>
       </c>
     </row>
@@ -3127,19 +3130,19 @@
       <c r="A15">
         <v>70</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>6.0316000000000001</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>-1.3137799999999999</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>2.1231</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>5.5014799999999999</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>6.5549899999999994E-2</v>
       </c>
     </row>
@@ -3147,19 +3150,19 @@
       <c r="A16">
         <v>75</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>8.1043299999999991</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>-1.9431400000000001</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>3.3128799999999998</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>7.1356000000000002</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>0.347244</v>
       </c>
     </row>
@@ -3167,19 +3170,19 @@
       <c r="A17">
         <v>80</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>10.5016</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>-2.3197100000000002</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>4.7057000000000002</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>8.95444</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>1.1132299999999999</v>
       </c>
     </row>
@@ -3187,19 +3190,19 @@
       <c r="A18">
         <v>85</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>13.1561</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>-2.07294</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>6.1773800000000003</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>10.796200000000001</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>2.3204600000000002</v>
       </c>
     </row>
@@ -3207,19 +3210,19 @@
       <c r="A19">
         <v>90</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>15.7981</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>-1.0748599999999999</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>7.5951199999999996</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>12.8361</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>3.5874600000000001</v>
       </c>
     </row>
@@ -3227,19 +3230,19 @@
       <c r="A20">
         <v>95</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>17.849599999999999</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>0.47650700000000001</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>8.8510299999999997</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>14.446400000000001</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>4.7776100000000001</v>
       </c>
     </row>
@@ -3247,19 +3250,19 @@
       <c r="A21">
         <v>100</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>18.7925</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>2.2438099999999999</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>9.8807700000000001</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>15.4047</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>5.8579600000000003</v>
       </c>
     </row>
@@ -3267,19 +3270,19 @@
       <c r="A22">
         <v>105</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>18.677600000000002</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>3.9555500000000001</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>10.666</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>15.576499999999999</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>6.8735799999999996</v>
       </c>
     </row>
@@ -3287,19 +3290,19 @@
       <c r="A23">
         <v>110</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>17.986899999999999</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>5.47248</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>11.224</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>15.408899999999999</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>7.72729</v>
       </c>
     </row>
@@ -3307,19 +3310,19 @@
       <c r="A24">
         <v>115</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>17.151</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>6.75481</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>11.593</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>15.0502</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>8.5320199999999993</v>
       </c>
     </row>
@@ -3327,19 +3330,19 @@
       <c r="A25">
         <v>120</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>16.368099999999998</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>7.8120700000000003</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>11.818199999999999</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>14.7202</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>9.1297099999999993</v>
       </c>
     </row>
@@ -3347,19 +3350,19 @@
       <c r="A26">
         <v>125</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>15.6877</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>8.6713699999999996</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>11.942299999999999</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>14.4177</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>9.70899</v>
       </c>
     </row>
@@ -3367,19 +3370,19 @@
       <c r="A27">
         <v>130</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>15.108000000000001</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>9.3630800000000001</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>12.0007</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>14.136200000000001</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>10.1173</v>
       </c>
     </row>
@@ -3387,19 +3390,19 @@
       <c r="A28">
         <v>135</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>14.6165</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>9.9157700000000002</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>12.0197</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>13.8841</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>10.5223</v>
       </c>
     </row>
@@ -3407,19 +3410,19 @@
       <c r="A29">
         <v>140</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>14.2006</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>10.3546</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>12.0174</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>13.6464</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>10.7826</v>
       </c>
     </row>
@@ -3427,19 +3430,19 @@
       <c r="A30">
         <v>145</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>13.8489</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>10.7012</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>12.0052</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>13.4115</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>11.0512</v>
       </c>
     </row>
@@ -3447,19 +3450,19 @@
       <c r="A31">
         <v>150</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>13.5517</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>10.973699999999999</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>11.989699999999999</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>13.193899999999999</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>11.215999999999999</v>
       </c>
     </row>
@@ -3467,19 +3470,19 @@
       <c r="A32">
         <v>155</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>13.300599999999999</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>11.186999999999999</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>11.9747</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>13.039400000000001</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>11.375</v>
       </c>
     </row>
@@ -3487,19 +3490,19 @@
       <c r="A33">
         <v>160</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>13.0886</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>11.353300000000001</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>11.961600000000001</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>12.8901</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>11.5052</v>
       </c>
     </row>
@@ -3507,19 +3510,19 @@
       <c r="A34">
         <v>165</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>12.909599999999999</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>11.482699999999999</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>11.950900000000001</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>12.7639</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>11.587899999999999</v>
       </c>
     </row>
@@ -3527,19 +3530,19 @@
       <c r="A35">
         <v>170</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>12.7584</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>11.583</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>11.942600000000001</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>12.645799999999999</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>11.6746</v>
       </c>
     </row>
@@ -3547,19 +3550,19 @@
       <c r="A36">
         <v>175</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>12.630800000000001</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>11.6607</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>11.936400000000001</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>12.532400000000001</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>11.7242</v>
       </c>
     </row>
@@ -3567,19 +3570,19 @@
       <c r="A37">
         <v>180</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>12.5229</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>11.720599999999999</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>11.931800000000001</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>12.455500000000001</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>11.767300000000001</v>
       </c>
     </row>
@@ -3587,19 +3590,19 @@
       <c r="A38">
         <v>185</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>12.431800000000001</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>11.7668</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>11.9284</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>12.385899999999999</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>11.810600000000001</v>
       </c>
     </row>
@@ -3607,19 +3610,19 @@
       <c r="A39">
         <v>190</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>12.354799999999999</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>11.8024</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>11.926</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>12.3049</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>11.830500000000001</v>
       </c>
     </row>
@@ -3627,19 +3630,19 @@
       <c r="A40">
         <v>195</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>12.2896</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>11.829800000000001</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>11.924300000000001</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>12.2575</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>11.8507</v>
       </c>
     </row>
@@ -3647,19 +3650,19 @@
       <c r="A41">
         <v>200</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>12.234500000000001</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>11.8508</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>11.9231</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>12.2117</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>11.8711</v>
       </c>
     </row>
@@ -3667,24 +3670,25 @@
       <c r="A42">
         <v>205</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>12.187799999999999</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>11.867000000000001</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>11.9222</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>12.1629</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>11.8803</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>